<commit_message>
Endpoint com exportacao de dados
</commit_message>
<xml_diff>
--- a/docs/excels/DesenhoLayout.xlsx
+++ b/docs/excels/DesenhoLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\Group-6\docs\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\PI\Group-6\docs\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9267D606-8A02-43F1-BBC4-29EAA7BBD15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D31325-89E6-40A8-80C3-FB668D6696DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76CEAE70-0381-46A9-B65E-1E533B98B9D8}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{76CEAE70-0381-46A9-B65E-1E533B98B9D8}"/>
   </bookViews>
   <sheets>
     <sheet name="HEADER" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,6 @@
     <t>Média</t>
   </si>
   <si>
-    <t>Media de valores poder dia</t>
-  </si>
-  <si>
     <t>72 - 72</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>Data prevista para terminar a campanha</t>
+  </si>
+  <si>
+    <t>Media de valores por dia</t>
   </si>
 </sst>
 </file>
@@ -330,15 +330,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E3C958-F98C-4DE4-965B-29447CF4C1EF}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,27 +675,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -705,7 +705,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -715,7 +715,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -725,7 +725,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1">
         <v>6</v>
@@ -735,7 +735,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -745,7 +745,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1">
         <v>45</v>
@@ -755,7 +755,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -765,7 +765,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="1">
         <v>19</v>
@@ -775,7 +775,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -785,7 +785,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -795,12 +795,12 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="4">
         <f>SUM(E2:E6)</f>
         <v>72</v>
@@ -819,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BBDCA7-CFB7-41F8-9F50-9AC11BC06332}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,292 +832,292 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>41</v>
+      <c r="F2" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>60</v>
+      <c r="B3" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1">
         <v>30</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>62</v>
-      </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1">
         <v>45</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>63</v>
+      <c r="F4" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1">
         <v>100</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>64</v>
+      <c r="F5" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>65</v>
+      <c r="F6" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1">
         <v>8</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1">
         <v>8</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>66</v>
+      <c r="F10" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1">
         <v>8</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1">
         <v>45</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1">
         <v>10</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>67</v>
+      <c r="F13" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1">
         <v>8</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>38</v>
+      <c r="F14" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="A15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="4">
         <f>SUM(E2:E14)</f>
         <v>287</v>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,27 +1148,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1178,17 +1178,17 @@
         <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1198,7 +1198,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1">
         <v>5</v>
@@ -1208,12 +1208,12 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="A4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="4">
         <f>SUM(E2:E3)</f>
         <v>6</v>

</xml_diff>